<commit_message>
Added new cases, updated README and assets
</commit_message>
<xml_diff>
--- a/data/20230131_list_violence_abductions_forced_conversions_hindu_women_in_pakistan.xlsx
+++ b/data/20230131_list_violence_abductions_forced_conversions_hindu_women_in_pakistan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Janak_Jain/Janak/Personal/projects/hindus_in_pakistan/github/hindus_in_pakistan/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3F6CDB7-EE1A-F443-A09D-146D00E7C449}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB3C53F1-3B47-4E48-BB89-4A62C189F849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{7834C0CA-90C6-1E41-85BA-104BC8C7D625}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AL$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AL$56</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="409">
   <si>
     <t>city</t>
   </si>
@@ -175,9 +175,6 @@
   </si>
   <si>
     <t>is_victim_reported_minor</t>
-  </si>
-  <si>
-    <t>victim_estimated_age</t>
   </si>
   <si>
     <t>victim_reported_age</t>
@@ -523,12 +520,6 @@
     <t>case_16</t>
   </si>
   <si>
-    <t>Matli</t>
-  </si>
-  <si>
-    <t>Tando Ghulam Ali: cases of abduction of minor Hindu girls #Nisha and #Hina have been closed due to false police reports and false challans.The girls have been handed over to kidnappers in Sindh.The Hindu community continues to face injustice and cruelty,but the government,courts.</t>
-  </si>
-  <si>
     <t>https://twitter.com/NarainDasBheel8/status/1613879349765181440?s=20&amp;t=EqQ5jcnK36bzUJy8PuZbAg</t>
   </si>
   <si>
@@ -542,9 +533,6 @@
   </si>
   <si>
     <t>Nisha</t>
-  </si>
-  <si>
-    <t>https://twitter.com/NarainDasBheel8/status/1613880668957573121?s=20&amp;t=EqQ5jcnK36bzUJy8PuZbAg</t>
   </si>
   <si>
     <t>Saveeta</t>
@@ -888,6 +876,483 @@
   </si>
   <si>
     <t>w/o Dina Bheel</t>
+  </si>
+  <si>
+    <t>case_31</t>
+  </si>
+  <si>
+    <t>Chanda</t>
+  </si>
+  <si>
+    <t>Shaneela</t>
+  </si>
+  <si>
+    <t>Tando Allahyar Sindh:
+A Hindu girl Shaneela from Tando Allahyar was forcefully converted to Islam and married to a Muslim man at Pir of Bharchiundi Shareef by Mian Javeed Ahmad Qadri.</t>
+  </si>
+  <si>
+    <t>https://twitter.com/NarainDasBheel8/status/1605204522208575488?s=20&amp;t=37g10exefm4l7cU-JhUmkg</t>
+  </si>
+  <si>
+    <t>case_32</t>
+  </si>
+  <si>
+    <t>Fateh Chowk</t>
+  </si>
+  <si>
+    <t>Hyderabad</t>
+  </si>
+  <si>
+    <t>victim_claimed_age</t>
+  </si>
+  <si>
+    <t>41304-4532420-3</t>
+  </si>
+  <si>
+    <t>Jamsi</t>
+  </si>
+  <si>
+    <t>case_33</t>
+  </si>
+  <si>
+    <t>Tando Ghulam Ali</t>
+  </si>
+  <si>
+    <t>Mustafa Dhokar, Shaukat Ali</t>
+  </si>
+  <si>
+    <t>A month ago in Chanda Maharaj case, her age was found to be 16 years in the verified report, after which the minor daughter was sent to a safe house and then in the new report with the help of the accused, the age was reported as 18 years, now she will be handed over to her</t>
+  </si>
+  <si>
+    <t>https://twitter.com/NarainDasBheel8/status/1603297389267374081?s=20&amp;t=37g10exefm4l7cU-JhUmkg</t>
+  </si>
+  <si>
+    <t>Pir Jan Srihandi</t>
+  </si>
+  <si>
+    <t>Samaru</t>
+  </si>
+  <si>
+    <t>NDTV</t>
+  </si>
+  <si>
+    <t>https://www.ndtv.com/world-news/pak-court-makes-decision-in-favour-of-man-who-abducted-hindu-girl-chanda-3453755</t>
+  </si>
+  <si>
+    <t>case_34</t>
+  </si>
+  <si>
+    <t>case_35</t>
+  </si>
+  <si>
+    <t>Salhepat Tehsil</t>
+  </si>
+  <si>
+    <t>Sukkur</t>
+  </si>
+  <si>
+    <t>Ood</t>
+  </si>
+  <si>
+    <t>Three Muslim men</t>
+  </si>
+  <si>
+    <t>case_36</t>
+  </si>
+  <si>
+    <t>Manzoor Shaikh</t>
+  </si>
+  <si>
+    <t>There used to be one way for girls belonging to religious minorities to avoid being kidnapped, forcibly converted to Islam, and married to Muslim men in Pakistan: getting married early. This is what Shanti Meghwar, from Tando Muhammad Khan in Southern Sindh, did. To no avail, as she has now been kidnapped by one Manzoor Shaikh and his friends. After having taken money from her parents for “expenses,” the police did not take any action.</t>
+  </si>
+  <si>
+    <t>BitterWinter</t>
+  </si>
+  <si>
+    <t>https://bitterwinter.org/pakistan-forced-conversions-of-hindu-girls/</t>
+  </si>
+  <si>
+    <t>case_37</t>
+  </si>
+  <si>
+    <t>Mustafa Dahokar</t>
+  </si>
+  <si>
+    <t>case_38</t>
+  </si>
+  <si>
+    <t>Dandari</t>
+  </si>
+  <si>
+    <t>Thatta</t>
+  </si>
+  <si>
+    <t>Salma</t>
+  </si>
+  <si>
+    <t>Shahid Unar</t>
+  </si>
+  <si>
+    <t>Salma Meghwar was abducted at gunpoint from her house in Dhandhari, near Thatta by Shahid Unar</t>
+  </si>
+  <si>
+    <t>case_39</t>
+  </si>
+  <si>
+    <t>Shalmi</t>
+  </si>
+  <si>
+    <t>case_40</t>
+  </si>
+  <si>
+    <t>case_41</t>
+  </si>
+  <si>
+    <t>Kareena</t>
+  </si>
+  <si>
+    <t>Sakina</t>
+  </si>
+  <si>
+    <t>Sakeena</t>
+  </si>
+  <si>
+    <t>Saleh Pat</t>
+  </si>
+  <si>
+    <t>case_42</t>
+  </si>
+  <si>
+    <t>Maya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ganghra Mori </t>
+  </si>
+  <si>
+    <t>Three people in car</t>
+  </si>
+  <si>
+    <t>https://twitter.com/NarainDasBheel8/status/1601213054481408000?s=20&amp;t=37g10exefm4l7cU-JhUmkg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hyderabad Sindh Pakistan 
+A 15-year-old minor Hindu Maya Kolhi, a resident of Hyderabad, was going to work with her mother, three people in an unknown white car were forcibly abducted  from Ganghra Mori </t>
+  </si>
+  <si>
+    <t>case_43</t>
+  </si>
+  <si>
+    <t>Pathani</t>
+  </si>
+  <si>
+    <t>Kunri Umarkot Sindh:
+Hindu woman Pathani Bheel who was forcefully converted to Islam, has been presented in Amarkot court. She told the Judge that she wants to go with her relatives, says she cannot stay away from her children.
+#StopForcedConversions</t>
+  </si>
+  <si>
+    <t>https://twitter.com/NarainDasBheel8/status/1601115138480041984?s=20&amp;t=37g10exefm4l7cU-JhUmkg</t>
+  </si>
+  <si>
+    <t>case_44</t>
+  </si>
+  <si>
+    <t>Wali</t>
+  </si>
+  <si>
+    <t>w/o Ramchand Meghwar</t>
+  </si>
+  <si>
+    <t>Mirpurkhas A married Hindu woman called Wali W/o Ramchand Meghwar was abducted and forcefully converted. Not only the woman, but her little boys Lov Kumar and Veer Kumar were also converted. Now will they produce certificate of little boys also falling in love with the abductor.</t>
+  </si>
+  <si>
+    <t>https://twitter.com/NarainDasBheel8/status/1599773190317694976?s=20&amp;t=37g10exefm4l7cU-JhUmkg</t>
+  </si>
+  <si>
+    <t>case_45</t>
+  </si>
+  <si>
+    <t>https://twitter.com/NarainDasBheel8/status/1598290090782261249?s=20&amp;t=37g10exefm4l7cU-JhUmkg</t>
+  </si>
+  <si>
+    <t>d/o Ramji Kolhi</t>
+  </si>
+  <si>
+    <t>Amna</t>
+  </si>
+  <si>
+    <t>Twitter, BitterWinter</t>
+  </si>
+  <si>
+    <t>https://twitter.com/NarainDasBheel8/status/1613880668957573121?s=20&amp;t=EqQ5jcnK36bzUJy8PuZbAg
+https://twitter.com/NarainDasBheel8/status/1599587905705742336?s=20&amp;t=37g10exefm4l7cU-JhUmkg
+https://bitterwinter.org/pakistan-forced-conversions-of-hindu-girls/</t>
+  </si>
+  <si>
+    <t>Narain Das Bheel, BitterWinter</t>
+  </si>
+  <si>
+    <t>Tando Bago</t>
+  </si>
+  <si>
+    <t>Tando Bago Badin Sindh 
+A Hindu girl Sakina d/o Walji has been abducted and converted into Islam.
+#StopForcedConversions
+#HinduLivesMatters
+#SaveMinoritiesInPakistan</t>
+  </si>
+  <si>
+    <t>https://twitter.com/NarainDasBheel8/status/1596451522216226817?s=20&amp;t=37g10exefm4l7cU-JhUmkg</t>
+  </si>
+  <si>
+    <t>d/o Walji</t>
+  </si>
+  <si>
+    <t>Kot Ghulam Muhammad Mirpurkhas Sindh:
+The mother of 4 children, a Hindu woman Shrimati Valki w/o Chetan Meghwar abducted and forcefully converted into islam and married to abductor,
+even after police complain police has not taken any action.
+#StopForcedConversions</t>
+  </si>
+  <si>
+    <t>Shrimate Valki</t>
+  </si>
+  <si>
+    <t>Kot Ghulam Muhammad</t>
+  </si>
+  <si>
+    <t>https://twitter.com/NarainDasBheel8/status/1596403558529716224?s=20&amp;t=37g10exefm4l7cU-JhUmkg</t>
+  </si>
+  <si>
+    <t>Kunri Umerkot Sindh:
+Geni w/o Kirshan bheel a Hindu woman who was abducted four months ago has succeed to escaped from kidnapper home she told she was gang r@ped and forcefully converted into Islam by Ali Gul kapri and others.
+#StopForcedConversions
+#saveminoritygirls</t>
+  </si>
+  <si>
+    <t>https://twitter.com/NarainDasBheel8/status/1596138058562162689?s=20&amp;t=37g10exefm4l7cU-JhUmkg</t>
+  </si>
+  <si>
+    <t>Ali Gur Kapri and others</t>
+  </si>
+  <si>
+    <t>case_46</t>
+  </si>
+  <si>
+    <t>Geni</t>
+  </si>
+  <si>
+    <t>w/o Kirshan Bheel</t>
+  </si>
+  <si>
+    <t>case_47</t>
+  </si>
+  <si>
+    <t>Mithi</t>
+  </si>
+  <si>
+    <t>Marvi</t>
+  </si>
+  <si>
+    <t>https://twitter.com/NarainDasBheel8/status/1595317492171345921?s=20&amp;t=37g10exefm4l7cU-JhUmkg</t>
+  </si>
+  <si>
+    <t>case_48</t>
+  </si>
+  <si>
+    <t>Pithoro</t>
+  </si>
+  <si>
+    <t>Jasodhan</t>
+  </si>
+  <si>
+    <t>Amnah</t>
+  </si>
+  <si>
+    <t>case_49</t>
+  </si>
+  <si>
+    <t>Jhuddo</t>
+  </si>
+  <si>
+    <t>Guddi</t>
+  </si>
+  <si>
+    <t>case_50</t>
+  </si>
+  <si>
+    <t>Amiyan</t>
+  </si>
+  <si>
+    <t>Pir Saiyan Agha Jan Sarhandi</t>
+  </si>
+  <si>
+    <t>Noor Nabi Samilejo</t>
+  </si>
+  <si>
+    <t>https://twitter.com/for_interfaith/status/1592883438008569859?s=20&amp;t=kgMZNN8-Y19BdSS7aozJWA</t>
+  </si>
+  <si>
+    <t>Another #ForcedConversion of #minorities in Sindh!!!!!
+A #Hindu girl Marvi Bheel has been forcefully converted into #Islam in Samaro by Pir Saiyan Agha Jan Sarhandi &amp; then forced to marry her own abductor Noor Nabi Samilejo.
+@GirlsNotBrides @HRCP87 @widhyarthi @amnesty</t>
+  </si>
+  <si>
+    <t>Wagherji, Kot Ghulam Muhammad</t>
+  </si>
+  <si>
+    <t>Naseem S/O Wahid Lagari</t>
+  </si>
+  <si>
+    <t>case_51</t>
+  </si>
+  <si>
+    <t>Hatki</t>
+  </si>
+  <si>
+    <t>Nagarparkar</t>
+  </si>
+  <si>
+    <t>D/O Shagan Meghwar</t>
+  </si>
+  <si>
+    <t>Mustafa Khaskhali</t>
+  </si>
+  <si>
+    <t>https://twitter.com/NarainDasBheel8/status/1594955915337285632?s=20&amp;t=PXlQgLWcK4X7gYJ_1_8zig</t>
+  </si>
+  <si>
+    <t>21-11-22 Nangarparkar Sindh:
+Mustafa Khaskhali abducted the married woman Hatki D/O Shagan Meghwar and forcefully converted her religion to Islam and got married. It looks nobody here who have some mercy We are citizens of this country and on top of that we are human too.
+#Hindus</t>
+  </si>
+  <si>
+    <t>case_52</t>
+  </si>
+  <si>
+    <t>Reema</t>
+  </si>
+  <si>
+    <t>Ali Hasan Lashari</t>
+  </si>
+  <si>
+    <t>Mother of three children. Already married</t>
+  </si>
+  <si>
+    <t>d/o Malomal Maharaj</t>
+  </si>
+  <si>
+    <t>Shaman Magsi Baloch and 3 others</t>
+  </si>
+  <si>
+    <t>http://fb.watch/g5081qTJPO/</t>
+  </si>
+  <si>
+    <t>d/o Mavji Kolhi</t>
+  </si>
+  <si>
+    <t>Abdul Rehman, Khoso, Matli</t>
+  </si>
+  <si>
+    <t>Sanaullah Malokh Dahokar</t>
+  </si>
+  <si>
+    <t>https://twitter.com/NarainDasBheel8/status/1613879349765181440?s=20&amp;t=EqQ5jcnK36bzUJy8PuZbAg
+http://fb.watch/gtDknNv1zp/</t>
+  </si>
+  <si>
+    <t>d/o Tanyo Kolhi</t>
+  </si>
+  <si>
+    <t>Ali Ghulam Tahim</t>
+  </si>
+  <si>
+    <t>https://twitter.com/NarainDasBheel8/status/1595317492171345921?s=20&amp;t=37g10exefm4l7cU-JhUmkg
+http://fb.watch/fWwJnc76yF/</t>
+  </si>
+  <si>
+    <t>Matli, Khoso colony, Tando Ghulam Ali</t>
+  </si>
+  <si>
+    <t>case_53</t>
+  </si>
+  <si>
+    <t>Karampur</t>
+  </si>
+  <si>
+    <t>Dadu</t>
+  </si>
+  <si>
+    <t>Anusha</t>
+  </si>
+  <si>
+    <t>case_54</t>
+  </si>
+  <si>
+    <t>Daani</t>
+  </si>
+  <si>
+    <t>Ayesha</t>
+  </si>
+  <si>
+    <t>Sheikh</t>
+  </si>
+  <si>
+    <t>https://twitter.com/NarainDasBheel8/status/1585984952625410048?s=20&amp;t=isLPbVxlaEpxA1s2P_eNbA</t>
+  </si>
+  <si>
+    <t>16-10-22 Kot Gulam Muhammad:Mirpurkhas Sindh 
+10 Mell mori A Hindu women name Daani D/o punhal kolhi mother of 4 kids has been converted to Islam and married to Zamaeer Hassan resident of Sui Gas. Her name changed from Dani to Ayesha Shaikh.
+#StopForcedConversions</t>
+  </si>
+  <si>
+    <t>D/o Punhal Kolhi</t>
+  </si>
+  <si>
+    <t>Zamaeer Hassan</t>
+  </si>
+  <si>
+    <t>case_55</t>
+  </si>
+  <si>
+    <t>Village Gorano, Islamkot</t>
+  </si>
+  <si>
+    <t>https://twitter.com/NarainDasBheel8/status/1594309096454336512?s=20&amp;t=37g10exefm4l7cU-JhUmkg</t>
+  </si>
+  <si>
+    <t>Tando Ghulam Ali: cases of abduction of minor Hindu girls #Nisha and #Hina have been closed due to false police reports and false challans.The girls have been handed over to kidnappers in Sindh.The Hindu community continues to face injustice and cruelty,but the government,courts.
+Born on Nov 11, 2011</t>
+  </si>
+  <si>
+    <t>Tando Ghulam Ali: cases of abduction of minor Hindu girls #Nisha and #Hina have been closed due to false police reports and false challans.The girls have been handed over to kidnappers in Sindh.The Hindu community continues to face injustice and cruelty,but the government,courts.
+On October 14 Hina Kolhi, a resident of Khosa Colony of Tando Ghulam Ali, was kidnapped, forcibly converted to Islam, and married to one Mustafa Dahokar.
+Cruelty and injustice to the Hindu community in Tandoghulam Ali Badin
+The hospital staff took a huge bribe from the criminals who kidnapped our daughters and handed over our 13-year-old innocent daughter #Hina to the accused as 19-year-old,which is complete cruelty and injustice
+Born on November 11, 2009</t>
+  </si>
+  <si>
+    <t>case_56</t>
+  </si>
+  <si>
+    <t>Maria</t>
+  </si>
+  <si>
+    <t>d/o Bagh Meghwar</t>
+  </si>
+  <si>
+    <t>https://twitter.com/NarainDasBheel8/status/1593554994371956736?s=20&amp;t=37g10exefm4l7cU-JhUmkg</t>
+  </si>
+  <si>
+    <t>A minor kid Maria, who was abducted from Kunbh in October 2022
+Parents revealed the name of the alleged kidnapper during the protest.
+Wazir wasan has abducted  a 10 y old minor girl Hindu Maria, police is not helping.
+#StopForcedConversions
+#saveminoritygirls</t>
+  </si>
+  <si>
+    <t>Kumb</t>
+  </si>
+  <si>
+    <t>Khairpur</t>
   </si>
 </sst>
 </file>
@@ -955,7 +1420,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -966,6 +1431,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1281,12 +1749,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D2FE676-F03D-4E4C-8907-AA9304B213EE}">
-  <dimension ref="A1:AL31"/>
+  <dimension ref="A1:AL57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1318,7 +1786,7 @@
         <v>5</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>27</v>
@@ -1333,10 +1801,10 @@
         <v>30</v>
       </c>
       <c r="M1" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="N1" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>46</v>
       </c>
       <c r="O1" s="4" t="s">
         <v>13</v>
@@ -1363,10 +1831,10 @@
         <v>42</v>
       </c>
       <c r="W1" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="X1" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Y1" s="4" t="s">
         <v>9</v>
@@ -1390,7 +1858,7 @@
         <v>14</v>
       </c>
       <c r="AF1" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AG1" s="4" t="s">
         <v>15</v>
@@ -1449,7 +1917,7 @@
         <v>20</v>
       </c>
       <c r="O2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="R2" t="b">
         <v>1</v>
@@ -1464,10 +1932,10 @@
         <v>0</v>
       </c>
       <c r="W2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="X2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Y2" t="b">
         <v>1</v>
@@ -1499,13 +1967,13 @@
     </row>
     <row r="3" spans="1:38" ht="102" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" t="s">
         <v>53</v>
-      </c>
-      <c r="B3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C3" t="s">
-        <v>54</v>
       </c>
       <c r="D3" t="s">
         <v>36</v>
@@ -1520,16 +1988,16 @@
         <v>44957</v>
       </c>
       <c r="I3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J3" t="s">
         <v>56</v>
-      </c>
-      <c r="J3" t="s">
-        <v>57</v>
       </c>
       <c r="M3">
         <v>11</v>
       </c>
       <c r="O3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="R3" t="b">
         <v>1</v>
@@ -1541,25 +2009,25 @@
         <v>0</v>
       </c>
       <c r="W3" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH3" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="Y3" t="b">
-        <v>1</v>
-      </c>
-      <c r="AB3" t="b">
-        <v>1</v>
-      </c>
-      <c r="AD3" t="b">
-        <v>1</v>
-      </c>
-      <c r="AH3" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="AI3" t="s">
         <v>21</v>
       </c>
       <c r="AJ3" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AL3" t="s">
         <v>24</v>
@@ -1567,10 +2035,10 @@
     </row>
     <row r="4" spans="1:38" ht="102" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" t="s">
         <v>62</v>
-      </c>
-      <c r="B4" t="s">
-        <v>63</v>
       </c>
       <c r="C4" t="s">
         <v>39</v>
@@ -1584,26 +2052,35 @@
       <c r="F4">
         <v>69.562719644697694</v>
       </c>
+      <c r="G4" s="2">
+        <v>44887</v>
+      </c>
       <c r="I4" t="s">
+        <v>63</v>
+      </c>
+      <c r="J4" t="s">
         <v>64</v>
       </c>
-      <c r="J4" t="s">
+      <c r="M4">
+        <v>6</v>
+      </c>
+      <c r="R4" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD4" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH4" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="R4" t="b">
-        <v>1</v>
-      </c>
-      <c r="AD4" t="b">
-        <v>1</v>
-      </c>
-      <c r="AH4" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="AI4" t="s">
         <v>21</v>
       </c>
       <c r="AJ4" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
+      </c>
+      <c r="AK4" s="3" t="s">
+        <v>324</v>
       </c>
       <c r="AL4" t="s">
         <v>24</v>
@@ -1611,7 +2088,7 @@
     </row>
     <row r="5" spans="1:38" ht="119" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C5" t="s">
         <v>35</v>
@@ -1623,31 +2100,31 @@
         <v>44954</v>
       </c>
       <c r="I5" t="s">
+        <v>68</v>
+      </c>
+      <c r="J5" t="s">
         <v>69</v>
       </c>
-      <c r="J5" t="s">
+      <c r="T5" t="b">
+        <v>1</v>
+      </c>
+      <c r="W5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AB5" t="b">
+        <v>1</v>
+      </c>
+      <c r="AE5" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH5" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="T5" t="b">
-        <v>1</v>
-      </c>
-      <c r="W5" t="s">
-        <v>72</v>
-      </c>
-      <c r="AB5" t="b">
-        <v>1</v>
-      </c>
-      <c r="AE5" t="b">
-        <v>1</v>
-      </c>
-      <c r="AH5" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="AI5" t="s">
         <v>21</v>
       </c>
       <c r="AJ5" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AL5" t="s">
         <v>24</v>
@@ -1655,13 +2132,13 @@
     </row>
     <row r="6" spans="1:38" ht="102" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" t="s">
         <v>73</v>
-      </c>
-      <c r="B6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C6" t="s">
-        <v>74</v>
       </c>
       <c r="D6" t="s">
         <v>36</v>
@@ -1676,16 +2153,16 @@
         <v>44952</v>
       </c>
       <c r="I6" t="s">
+        <v>75</v>
+      </c>
+      <c r="J6" t="s">
         <v>76</v>
-      </c>
-      <c r="J6" t="s">
-        <v>77</v>
       </c>
       <c r="N6">
         <v>20</v>
       </c>
       <c r="O6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="S6" t="b">
         <v>0</v>
@@ -1700,22 +2177,22 @@
         <v>1</v>
       </c>
       <c r="Z6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AA6" t="s">
         <v>78</v>
       </c>
-      <c r="AA6" t="s">
+      <c r="AB6" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH6" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="AB6" t="b">
-        <v>1</v>
-      </c>
-      <c r="AH6" s="1" t="s">
-        <v>80</v>
       </c>
       <c r="AI6" t="s">
         <v>21</v>
       </c>
       <c r="AJ6" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AL6" t="s">
         <v>24</v>
@@ -1723,13 +2200,13 @@
     </row>
     <row r="7" spans="1:38" ht="136" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" t="s">
         <v>85</v>
-      </c>
-      <c r="C7" t="s">
-        <v>86</v>
       </c>
       <c r="D7" t="s">
         <v>36</v>
@@ -1744,7 +2221,7 @@
         <v>44948</v>
       </c>
       <c r="I7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J7" t="s">
         <v>33</v>
@@ -1756,13 +2233,13 @@
         <v>1</v>
       </c>
       <c r="AH7" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AI7" t="s">
         <v>21</v>
       </c>
       <c r="AJ7" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AL7" t="s">
         <v>24</v>
@@ -1770,10 +2247,10 @@
     </row>
     <row r="8" spans="1:38" ht="187" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C8" t="s">
         <v>39</v>
@@ -1797,10 +2274,10 @@
         <v>1</v>
       </c>
       <c r="V8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="W8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AB8" t="b">
         <v>0</v>
@@ -1815,21 +2292,21 @@
         <v>1</v>
       </c>
       <c r="AH8" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AI8" t="s">
         <v>21</v>
       </c>
       <c r="AJ8" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="AL8" t="s">
         <v>88</v>
-      </c>
-      <c r="AL8" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:38" ht="136" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C9" t="s">
         <v>39</v>
@@ -1847,10 +2324,10 @@
         <v>44545</v>
       </c>
       <c r="I9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="T9" t="b">
         <v>1</v>
@@ -1859,33 +2336,33 @@
         <v>1</v>
       </c>
       <c r="V9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AB9" t="b">
         <v>0</v>
       </c>
       <c r="AH9" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AI9" t="s">
         <v>21</v>
       </c>
       <c r="AJ9" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="AK9" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="AL9" t="s">
         <v>95</v>
-      </c>
-      <c r="AK9" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="AL9" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:38" ht="119" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C10" t="s">
         <v>39</v>
@@ -1903,19 +2380,19 @@
         <v>45285</v>
       </c>
       <c r="I10" t="s">
+        <v>101</v>
+      </c>
+      <c r="J10" t="s">
         <v>102</v>
       </c>
-      <c r="J10" t="s">
+      <c r="P10" t="s">
+        <v>155</v>
+      </c>
+      <c r="T10" t="b">
+        <v>1</v>
+      </c>
+      <c r="W10" t="s">
         <v>103</v>
-      </c>
-      <c r="P10" t="s">
-        <v>158</v>
-      </c>
-      <c r="T10" t="b">
-        <v>1</v>
-      </c>
-      <c r="W10" t="s">
-        <v>104</v>
       </c>
       <c r="Y10" t="b">
         <v>1</v>
@@ -1936,16 +2413,16 @@
         <v>1</v>
       </c>
       <c r="AH10" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AI10" t="s">
         <v>21</v>
       </c>
       <c r="AJ10" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AK10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AL10" t="s">
         <v>24</v>
@@ -1953,13 +2430,13 @@
     </row>
     <row r="11" spans="1:38" ht="68" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>106</v>
+      </c>
+      <c r="B11" t="s">
         <v>107</v>
       </c>
-      <c r="B11" t="s">
-        <v>108</v>
-      </c>
       <c r="C11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D11" t="s">
         <v>36</v>
@@ -1974,16 +2451,16 @@
         <v>44909</v>
       </c>
       <c r="I11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J11" t="s">
         <v>33</v>
       </c>
       <c r="P11" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q11" t="s">
         <v>110</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>111</v>
       </c>
       <c r="T11" t="b">
         <v>0</v>
@@ -1992,22 +2469,22 @@
         <v>1</v>
       </c>
       <c r="V11" t="s">
+        <v>111</v>
+      </c>
+      <c r="W11" t="s">
         <v>112</v>
       </c>
-      <c r="W11" t="s">
-        <v>113</v>
-      </c>
       <c r="AB11" t="b">
         <v>1</v>
       </c>
       <c r="AH11" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AI11" t="s">
         <v>21</v>
       </c>
       <c r="AJ11" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AL11" t="s">
         <v>24</v>
@@ -2015,10 +2492,10 @@
     </row>
     <row r="12" spans="1:38" ht="136" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D12" t="s">
         <v>36</v>
@@ -2027,28 +2504,28 @@
         <v>44947</v>
       </c>
       <c r="I12" t="s">
+        <v>117</v>
+      </c>
+      <c r="J12" t="s">
+        <v>64</v>
+      </c>
+      <c r="P12" t="s">
         <v>118</v>
       </c>
-      <c r="J12" t="s">
-        <v>65</v>
-      </c>
-      <c r="P12" t="s">
+      <c r="Q12" t="s">
+        <v>110</v>
+      </c>
+      <c r="T12" t="b">
+        <v>1</v>
+      </c>
+      <c r="U12" t="b">
+        <v>1</v>
+      </c>
+      <c r="V12" t="s">
         <v>119</v>
       </c>
-      <c r="Q12" t="s">
-        <v>111</v>
-      </c>
-      <c r="T12" t="b">
-        <v>1</v>
-      </c>
-      <c r="U12" t="b">
-        <v>1</v>
-      </c>
-      <c r="V12" t="s">
+      <c r="W12" t="s">
         <v>120</v>
-      </c>
-      <c r="W12" t="s">
-        <v>121</v>
       </c>
       <c r="Y12" t="b">
         <v>1</v>
@@ -2063,16 +2540,16 @@
         <v>1</v>
       </c>
       <c r="AH12" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AI12" t="s">
         <v>21</v>
       </c>
       <c r="AJ12" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="AK12" s="3" t="s">
         <v>123</v>
-      </c>
-      <c r="AK12" s="3" t="s">
-        <v>124</v>
       </c>
       <c r="AL12" t="s">
         <v>24</v>
@@ -2080,13 +2557,13 @@
     </row>
     <row r="13" spans="1:38" ht="119" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B13" t="s">
+        <v>126</v>
+      </c>
+      <c r="C13" t="s">
         <v>125</v>
-      </c>
-      <c r="B13" t="s">
-        <v>127</v>
-      </c>
-      <c r="C13" t="s">
-        <v>126</v>
       </c>
       <c r="D13" t="s">
         <v>36</v>
@@ -2101,25 +2578,25 @@
         <v>44942</v>
       </c>
       <c r="J13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K13" t="s">
+        <v>127</v>
+      </c>
+      <c r="R13" t="b">
+        <v>1</v>
+      </c>
+      <c r="T13" t="b">
+        <v>1</v>
+      </c>
+      <c r="W13" t="s">
         <v>128</v>
       </c>
-      <c r="R13" t="b">
-        <v>1</v>
-      </c>
-      <c r="T13" t="b">
-        <v>1</v>
-      </c>
-      <c r="W13" t="s">
+      <c r="Y13" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z13" t="s">
         <v>129</v>
-      </c>
-      <c r="Y13" t="b">
-        <v>1</v>
-      </c>
-      <c r="Z13" t="s">
-        <v>130</v>
       </c>
       <c r="AB13" t="b">
         <v>1</v>
@@ -2134,13 +2611,13 @@
         <v>1</v>
       </c>
       <c r="AH13" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AI13" t="s">
         <v>21</v>
       </c>
       <c r="AJ13" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AL13" t="s">
         <v>24</v>
@@ -2148,13 +2625,13 @@
     </row>
     <row r="14" spans="1:38" ht="170" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B14" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D14" t="s">
         <v>36</v>
@@ -2169,19 +2646,19 @@
         <v>44923</v>
       </c>
       <c r="H14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I14" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="J14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="P14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="Q14" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="R14" t="b">
         <v>0</v>
@@ -2196,16 +2673,16 @@
         <v>1</v>
       </c>
       <c r="AH14" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AI14" t="s">
         <v>21</v>
       </c>
       <c r="AJ14" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AK14" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="AL14" t="s">
         <v>24</v>
@@ -2213,13 +2690,13 @@
     </row>
     <row r="15" spans="1:38" ht="119" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B15" t="s">
+        <v>139</v>
+      </c>
+      <c r="C15" t="s">
         <v>140</v>
-      </c>
-      <c r="C15" t="s">
-        <v>141</v>
       </c>
       <c r="D15" t="s">
         <v>36</v>
@@ -2231,16 +2708,16 @@
         <v>69.411348052444694</v>
       </c>
       <c r="I15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="P15" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q15" t="s">
         <v>145</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>146</v>
       </c>
       <c r="R15" t="b">
         <v>0</v>
@@ -2255,7 +2732,7 @@
         <v>1</v>
       </c>
       <c r="W15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="Y15" t="b">
         <v>1</v>
@@ -2264,13 +2741,13 @@
         <v>0</v>
       </c>
       <c r="AH15" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AI15" t="s">
         <v>21</v>
       </c>
       <c r="AJ15" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AL15" t="s">
         <v>24</v>
@@ -2278,13 +2755,13 @@
     </row>
     <row r="16" spans="1:38" ht="136" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C16" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D16" t="s">
         <v>36</v>
@@ -2299,7 +2776,7 @@
         <v>44934</v>
       </c>
       <c r="I16" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="J16" t="s">
         <v>33</v>
@@ -2311,7 +2788,7 @@
         <v>19</v>
       </c>
       <c r="P16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="R16" t="b">
         <v>1</v>
@@ -2320,7 +2797,7 @@
         <v>0</v>
       </c>
       <c r="W16" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="Y16" t="b">
         <v>1</v>
@@ -2338,27 +2815,27 @@
         <v>1</v>
       </c>
       <c r="AH16" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AI16" t="s">
         <v>21</v>
       </c>
       <c r="AJ16" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="AK16" s="3" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="AL16" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:38" ht="119" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:38" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B17" t="s">
-        <v>155</v>
+        <v>384</v>
       </c>
       <c r="C17" t="s">
         <v>35</v>
@@ -2373,13 +2850,25 @@
         <v>68.660286746199205</v>
       </c>
       <c r="G17" s="2">
-        <v>44898</v>
+        <v>44848</v>
       </c>
       <c r="I17" t="s">
-        <v>159</v>
+        <v>156</v>
+      </c>
+      <c r="J17" t="s">
+        <v>325</v>
+      </c>
+      <c r="K17" t="s">
+        <v>326</v>
+      </c>
+      <c r="M17">
+        <v>13</v>
+      </c>
+      <c r="N17">
+        <v>19</v>
       </c>
       <c r="P17" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="R17" t="b">
         <v>1</v>
@@ -2390,6 +2879,9 @@
       <c r="T17" t="b">
         <v>1</v>
       </c>
+      <c r="W17" t="s">
+        <v>293</v>
+      </c>
       <c r="Y17" t="b">
         <v>1</v>
       </c>
@@ -2406,27 +2898,27 @@
         <v>1</v>
       </c>
       <c r="AH17" s="1" t="s">
-        <v>156</v>
+        <v>401</v>
       </c>
       <c r="AI17" t="s">
-        <v>21</v>
+        <v>327</v>
       </c>
       <c r="AJ17" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="AK17" s="6" t="s">
+        <v>328</v>
+      </c>
+      <c r="AL17" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="18" spans="1:38" ht="238" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>157</v>
       </c>
-      <c r="AK17" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="AL17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:38" ht="119" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>160</v>
-      </c>
       <c r="B18" t="s">
-        <v>155</v>
+        <v>378</v>
       </c>
       <c r="C18" t="s">
         <v>35</v>
@@ -2440,11 +2932,26 @@
       <c r="F18">
         <v>68.660286746199205</v>
       </c>
+      <c r="G18" s="2">
+        <v>44830</v>
+      </c>
       <c r="I18" t="s">
-        <v>161</v>
+        <v>158</v>
+      </c>
+      <c r="J18" t="s">
+        <v>377</v>
+      </c>
+      <c r="K18" t="s">
+        <v>242</v>
+      </c>
+      <c r="M18">
+        <v>11</v>
+      </c>
+      <c r="N18">
+        <v>16</v>
       </c>
       <c r="P18" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="R18" t="b">
         <v>1</v>
@@ -2452,6 +2959,9 @@
       <c r="T18" t="b">
         <v>1</v>
       </c>
+      <c r="W18" t="s">
+        <v>379</v>
+      </c>
       <c r="Y18" t="b">
         <v>1</v>
       </c>
@@ -2468,13 +2978,13 @@
         <v>1</v>
       </c>
       <c r="AH18" s="1" t="s">
-        <v>156</v>
+        <v>400</v>
       </c>
       <c r="AI18" t="s">
         <v>21</v>
       </c>
-      <c r="AJ18" s="3" t="s">
-        <v>157</v>
+      <c r="AJ18" s="6" t="s">
+        <v>380</v>
       </c>
       <c r="AL18" t="s">
         <v>24</v>
@@ -2482,10 +2992,10 @@
     </row>
     <row r="19" spans="1:38" ht="85" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C19" t="s">
         <v>39</v>
@@ -2503,16 +3013,16 @@
         <v>44921</v>
       </c>
       <c r="I19" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="J19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="P19" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="Q19" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="R19" t="b">
         <v>0</v>
@@ -2521,19 +3031,19 @@
         <v>0</v>
       </c>
       <c r="W19" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="AD19" t="b">
         <v>1</v>
       </c>
       <c r="AH19" s="1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="AI19" t="s">
         <v>21</v>
       </c>
       <c r="AJ19" s="3" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="AL19" t="s">
         <v>24</v>
@@ -2541,13 +3051,13 @@
     </row>
     <row r="20" spans="1:38" ht="136" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B20" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C20" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="D20" t="s">
         <v>36</v>
@@ -2562,22 +3072,22 @@
         <v>44914</v>
       </c>
       <c r="I20" t="s">
+        <v>170</v>
+      </c>
+      <c r="J20" t="s">
+        <v>171</v>
+      </c>
+      <c r="K20" t="s">
         <v>174</v>
       </c>
-      <c r="J20" t="s">
+      <c r="L20" t="s">
         <v>175</v>
-      </c>
-      <c r="K20" t="s">
-        <v>178</v>
-      </c>
-      <c r="L20" t="s">
-        <v>179</v>
       </c>
       <c r="M20">
         <v>15</v>
       </c>
       <c r="P20" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="R20" t="b">
         <v>1</v>
@@ -2586,7 +3096,7 @@
         <v>1</v>
       </c>
       <c r="W20" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="Y20" t="b">
         <v>1</v>
@@ -2598,13 +3108,13 @@
         <v>1</v>
       </c>
       <c r="AH20" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="AI20" t="s">
         <v>21</v>
       </c>
       <c r="AJ20" s="3" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="AL20" t="s">
         <v>24</v>
@@ -2612,13 +3122,13 @@
     </row>
     <row r="21" spans="1:38" ht="136" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B21" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C21" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="D21" t="s">
         <v>36</v>
@@ -2633,10 +3143,10 @@
         <v>44784</v>
       </c>
       <c r="P21" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="Q21" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="T21" t="b">
         <v>1</v>
@@ -2651,13 +3161,13 @@
         <v>1</v>
       </c>
       <c r="AH21" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="AI21" t="s">
         <v>21</v>
       </c>
       <c r="AJ21" s="3" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="AL21" t="s">
         <v>24</v>
@@ -2665,16 +3175,16 @@
     </row>
     <row r="22" spans="1:38" ht="119" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B22" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C22" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="D22" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E22">
         <v>29.5557738233809</v>
@@ -2686,52 +3196,52 @@
         <v>44201</v>
       </c>
       <c r="I22" t="s">
+        <v>186</v>
+      </c>
+      <c r="J22" t="s">
+        <v>187</v>
+      </c>
+      <c r="K22" t="s">
+        <v>192</v>
+      </c>
+      <c r="P22" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>180</v>
+      </c>
+      <c r="T22" t="b">
+        <v>1</v>
+      </c>
+      <c r="W22" t="s">
         <v>190</v>
       </c>
-      <c r="J22" t="s">
+      <c r="Y22" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>189</v>
+      </c>
+      <c r="AB22" t="b">
+        <v>1</v>
+      </c>
+      <c r="AC22" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD22" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH22" s="1" t="s">
         <v>191</v>
-      </c>
-      <c r="K22" t="s">
-        <v>196</v>
-      </c>
-      <c r="P22" t="s">
-        <v>158</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>184</v>
-      </c>
-      <c r="T22" t="b">
-        <v>1</v>
-      </c>
-      <c r="W22" t="s">
-        <v>194</v>
-      </c>
-      <c r="Y22" t="b">
-        <v>1</v>
-      </c>
-      <c r="Z22" t="s">
-        <v>193</v>
-      </c>
-      <c r="AB22" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC22" t="b">
-        <v>1</v>
-      </c>
-      <c r="AD22" t="b">
-        <v>1</v>
-      </c>
-      <c r="AH22" s="1" t="s">
-        <v>195</v>
       </c>
       <c r="AI22" t="s">
         <v>21</v>
       </c>
       <c r="AJ22" s="3" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="AK22" s="3" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="AL22" t="s">
         <v>24</v>
@@ -2739,13 +3249,13 @@
     </row>
     <row r="23" spans="1:38" ht="238" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B23" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C23" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D23" t="s">
         <v>36</v>
@@ -2760,19 +3270,19 @@
         <v>44933</v>
       </c>
       <c r="I23" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="J23" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="N23">
         <v>22</v>
       </c>
       <c r="P23" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="Q23" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="S23" t="b">
         <v>0</v>
@@ -2781,22 +3291,22 @@
         <v>1</v>
       </c>
       <c r="V23" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="Y23" t="b">
         <v>0</v>
       </c>
       <c r="AH23" s="1" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="AI23" t="s">
         <v>21</v>
       </c>
       <c r="AJ23" s="3" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="AK23" s="5" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="AL23" t="s">
         <v>24</v>
@@ -2804,13 +3314,13 @@
     </row>
     <row r="24" spans="1:38" ht="119" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>201</v>
+      </c>
+      <c r="B24" t="s">
         <v>205</v>
       </c>
-      <c r="B24" t="s">
-        <v>209</v>
-      </c>
       <c r="C24" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="D24" t="s">
         <v>36</v>
@@ -2825,16 +3335,16 @@
         <v>44933</v>
       </c>
       <c r="I24" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="J24" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="P24" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="Q24" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="T24" t="b">
         <v>1</v>
@@ -2843,22 +3353,22 @@
         <v>1</v>
       </c>
       <c r="V24" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="Y24" t="b">
         <v>0</v>
       </c>
       <c r="AH24" s="1" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="AI24" t="s">
         <v>21</v>
       </c>
       <c r="AJ24" s="3" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="AK24" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="AL24" t="s">
         <v>24</v>
@@ -2866,13 +3376,13 @@
     </row>
     <row r="25" spans="1:38" ht="119" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="B25" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C25" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="D25" t="s">
         <v>36</v>
@@ -2887,16 +3397,16 @@
         <v>44933</v>
       </c>
       <c r="I25" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="J25" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="P25" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="Q25" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="T25" t="b">
         <v>1</v>
@@ -2905,22 +3415,22 @@
         <v>1</v>
       </c>
       <c r="V25" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="Y25" t="b">
         <v>0</v>
       </c>
       <c r="AH25" s="1" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="AI25" t="s">
         <v>21</v>
       </c>
       <c r="AJ25" s="3" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="AK25" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="AL25" t="s">
         <v>24</v>
@@ -2928,13 +3438,13 @@
     </row>
     <row r="26" spans="1:38" ht="136" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="B26" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C26" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="D26" t="s">
         <v>36</v>
@@ -2949,10 +3459,10 @@
         <v>44667</v>
       </c>
       <c r="I26" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="J26" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="M26">
         <v>14</v>
@@ -2961,10 +3471,10 @@
         <v>18</v>
       </c>
       <c r="P26" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="Q26" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="R26" t="b">
         <v>1</v>
@@ -2973,13 +3483,13 @@
         <v>0</v>
       </c>
       <c r="W26" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="Y26" t="b">
         <v>1</v>
       </c>
       <c r="Z26" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="AB26" t="b">
         <v>1</v>
@@ -2997,16 +3507,16 @@
         <v>1</v>
       </c>
       <c r="AH26" s="1" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="AI26" t="s">
         <v>21</v>
       </c>
       <c r="AJ26" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="AK26" s="3" t="s">
         <v>219</v>
-      </c>
-      <c r="AK26" s="3" t="s">
-        <v>223</v>
       </c>
       <c r="AL26" t="s">
         <v>24</v>
@@ -3014,13 +3524,13 @@
     </row>
     <row r="27" spans="1:38" ht="136" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="B27" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C27" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="D27" t="s">
         <v>36</v>
@@ -3035,19 +3545,19 @@
         <v>44932</v>
       </c>
       <c r="I27" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="J27" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="M27">
         <v>14</v>
       </c>
       <c r="P27" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="Q27" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="R27" t="b">
         <v>1</v>
@@ -3059,13 +3569,13 @@
         <v>1</v>
       </c>
       <c r="AH27" s="1" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="AI27" t="s">
         <v>21</v>
       </c>
       <c r="AJ27" s="3" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="AL27" t="s">
         <v>24</v>
@@ -3073,13 +3583,13 @@
     </row>
     <row r="28" spans="1:38" ht="153" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B28" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D28" t="s">
         <v>36</v>
@@ -3094,22 +3604,22 @@
         <v>44931</v>
       </c>
       <c r="I28" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="J28" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="M28">
         <v>12</v>
       </c>
       <c r="P28" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="R28" t="b">
         <v>1</v>
       </c>
       <c r="W28" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="AB28" t="b">
         <v>1</v>
@@ -3118,13 +3628,13 @@
         <v>1</v>
       </c>
       <c r="AH28" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="AI28" t="s">
         <v>21</v>
       </c>
       <c r="AJ28" s="3" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="AL28" t="s">
         <v>24</v>
@@ -3132,31 +3642,31 @@
     </row>
     <row r="29" spans="1:38" ht="119" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="G29" s="2">
         <v>44930</v>
       </c>
       <c r="I29" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="J29" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="K29" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="L29" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="N29">
         <v>23</v>
       </c>
       <c r="P29" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="Q29" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="S29" t="b">
         <v>0</v>
@@ -3168,10 +3678,10 @@
         <v>1</v>
       </c>
       <c r="Z29" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AA29" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="AB29" t="b">
         <v>1</v>
@@ -3183,13 +3693,13 @@
         <v>1</v>
       </c>
       <c r="AH29" s="1" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="AI29" t="s">
         <v>21</v>
       </c>
       <c r="AJ29" s="3" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="AL29" t="s">
         <v>24</v>
@@ -3197,13 +3707,13 @@
     </row>
     <row r="30" spans="1:38" ht="187" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B30" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C30" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="D30" t="s">
         <v>36</v>
@@ -3218,10 +3728,10 @@
         <v>44915</v>
       </c>
       <c r="I30" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="J30" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="M30">
         <v>13</v>
@@ -3230,10 +3740,10 @@
         <v>13</v>
       </c>
       <c r="P30" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="Q30" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="R30" t="b">
         <v>1</v>
@@ -3242,7 +3752,7 @@
         <v>1</v>
       </c>
       <c r="W30" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="Y30" t="b">
         <v>1</v>
@@ -3257,13 +3767,13 @@
         <v>1</v>
       </c>
       <c r="AH30" s="1" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="AI30" t="s">
         <v>21</v>
       </c>
       <c r="AJ30" s="3" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="AL30" t="s">
         <v>24</v>
@@ -3271,16 +3781,16 @@
     </row>
     <row r="31" spans="1:38" ht="153" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>253</v>
+      </c>
+      <c r="B31" t="s">
+        <v>256</v>
+      </c>
+      <c r="C31" t="s">
         <v>257</v>
       </c>
-      <c r="B31" t="s">
-        <v>260</v>
-      </c>
-      <c r="C31" t="s">
-        <v>261</v>
-      </c>
       <c r="D31" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="E31">
         <v>28.260044969103699</v>
@@ -3292,16 +3802,16 @@
         <v>44918</v>
       </c>
       <c r="I31" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="J31" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="P31" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="Q31" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="R31" t="b">
         <v>0</v>
@@ -3310,10 +3820,10 @@
         <v>1</v>
       </c>
       <c r="Z31" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AA31" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="AC31" t="b">
         <v>1</v>
@@ -3322,20 +3832,1557 @@
         <v>1</v>
       </c>
       <c r="AH31" s="1" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="AI31" t="s">
         <v>21</v>
       </c>
       <c r="AJ31" s="3" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="AL31" t="s">
         <v>24</v>
       </c>
     </row>
+    <row r="32" spans="1:38" ht="102" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>261</v>
+      </c>
+      <c r="C32" t="s">
+        <v>125</v>
+      </c>
+      <c r="D32" t="s">
+        <v>36</v>
+      </c>
+      <c r="E32">
+        <v>25.457666548486799</v>
+      </c>
+      <c r="F32">
+        <v>68.722068683640799</v>
+      </c>
+      <c r="G32" s="2">
+        <v>44915</v>
+      </c>
+      <c r="I32" t="s">
+        <v>263</v>
+      </c>
+      <c r="P32" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>180</v>
+      </c>
+      <c r="Y32" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z32" t="s">
+        <v>77</v>
+      </c>
+      <c r="AA32" t="s">
+        <v>244</v>
+      </c>
+      <c r="AC32" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD32" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH32" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="AI32" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ32" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="AL32" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:38" ht="119" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>266</v>
+      </c>
+      <c r="B33" t="s">
+        <v>267</v>
+      </c>
+      <c r="C33" t="s">
+        <v>268</v>
+      </c>
+      <c r="D33" t="s">
+        <v>36</v>
+      </c>
+      <c r="E33">
+        <v>25.3839117149138</v>
+      </c>
+      <c r="F33">
+        <v>68.3676165029337</v>
+      </c>
+      <c r="G33" s="2">
+        <v>44785</v>
+      </c>
+      <c r="H33" t="s">
+        <v>270</v>
+      </c>
+      <c r="I33" t="s">
+        <v>262</v>
+      </c>
+      <c r="J33" t="s">
+        <v>374</v>
+      </c>
+      <c r="M33">
+        <v>13</v>
+      </c>
+      <c r="N33">
+        <v>18</v>
+      </c>
+      <c r="P33" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>180</v>
+      </c>
+      <c r="R33" t="b">
+        <v>1</v>
+      </c>
+      <c r="S33" t="b">
+        <v>0</v>
+      </c>
+      <c r="T33" t="b">
+        <v>1</v>
+      </c>
+      <c r="U33" t="b">
+        <v>1</v>
+      </c>
+      <c r="V33" t="s">
+        <v>110</v>
+      </c>
+      <c r="W33" t="s">
+        <v>375</v>
+      </c>
+      <c r="Y33" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB33" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD33" t="b">
+        <v>1</v>
+      </c>
+      <c r="AE33" t="b">
+        <v>1</v>
+      </c>
+      <c r="AF33" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH33" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="AI33" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ33" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="AK33" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="AL33" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>272</v>
+      </c>
+      <c r="B34" t="s">
+        <v>273</v>
+      </c>
+      <c r="C34" t="s">
+        <v>73</v>
+      </c>
+      <c r="D34" t="s">
+        <v>36</v>
+      </c>
+      <c r="E34">
+        <v>25.124136176544901</v>
+      </c>
+      <c r="F34">
+        <v>68.891752999995205</v>
+      </c>
+      <c r="G34" s="2">
+        <v>44854</v>
+      </c>
+      <c r="I34" t="s">
+        <v>271</v>
+      </c>
+      <c r="J34" t="s">
+        <v>33</v>
+      </c>
+      <c r="M34">
+        <v>14</v>
+      </c>
+      <c r="P34" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>180</v>
+      </c>
+      <c r="R34" t="b">
+        <v>1</v>
+      </c>
+      <c r="T34" t="b">
+        <v>1</v>
+      </c>
+      <c r="W34" t="s">
+        <v>274</v>
+      </c>
+      <c r="Y34" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z34" t="s">
+        <v>278</v>
+      </c>
+      <c r="AA34" t="s">
+        <v>277</v>
+      </c>
+      <c r="AC34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AE34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AF34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI34" t="s">
+        <v>279</v>
+      </c>
+      <c r="AJ34" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="AL34" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="35" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>281</v>
+      </c>
+      <c r="B35" t="s">
+        <v>283</v>
+      </c>
+      <c r="C35" t="s">
+        <v>284</v>
+      </c>
+      <c r="D35" t="s">
+        <v>36</v>
+      </c>
+      <c r="E35">
+        <v>27.343571971153999</v>
+      </c>
+      <c r="F35">
+        <v>69.305841420118895</v>
+      </c>
+      <c r="G35" s="2">
+        <v>44853</v>
+      </c>
+      <c r="I35" t="s">
+        <v>210</v>
+      </c>
+      <c r="J35" t="s">
+        <v>211</v>
+      </c>
+      <c r="M35">
+        <v>17</v>
+      </c>
+      <c r="O35" t="s">
+        <v>285</v>
+      </c>
+      <c r="P35" t="s">
+        <v>152</v>
+      </c>
+      <c r="R35" t="b">
+        <v>1</v>
+      </c>
+      <c r="W35" t="s">
+        <v>286</v>
+      </c>
+      <c r="AD35" t="b">
+        <v>1</v>
+      </c>
+      <c r="AE35" t="b">
+        <v>1</v>
+      </c>
+      <c r="AF35" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI35" t="s">
+        <v>279</v>
+      </c>
+      <c r="AJ35" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="AL35" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="36" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>282</v>
+      </c>
+      <c r="B36" t="s">
+        <v>283</v>
+      </c>
+      <c r="C36" t="s">
+        <v>284</v>
+      </c>
+      <c r="D36" t="s">
+        <v>36</v>
+      </c>
+      <c r="E36">
+        <v>27.343571971153999</v>
+      </c>
+      <c r="F36">
+        <v>69.305841420118895</v>
+      </c>
+      <c r="G36" s="2">
+        <v>44853</v>
+      </c>
+      <c r="I36" t="s">
+        <v>210</v>
+      </c>
+      <c r="J36" t="s">
+        <v>212</v>
+      </c>
+      <c r="M36">
+        <v>18</v>
+      </c>
+      <c r="O36" t="s">
+        <v>285</v>
+      </c>
+      <c r="P36" t="s">
+        <v>152</v>
+      </c>
+      <c r="R36" t="b">
+        <v>0</v>
+      </c>
+      <c r="W36" t="s">
+        <v>286</v>
+      </c>
+      <c r="AD36" t="b">
+        <v>1</v>
+      </c>
+      <c r="AE36" t="b">
+        <v>1</v>
+      </c>
+      <c r="AF36" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI36" t="s">
+        <v>279</v>
+      </c>
+      <c r="AJ36" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="AL36" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="37" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>287</v>
+      </c>
+      <c r="C37" t="s">
+        <v>179</v>
+      </c>
+      <c r="D37" t="s">
+        <v>36</v>
+      </c>
+      <c r="E37">
+        <v>25.126696706324701</v>
+      </c>
+      <c r="F37">
+        <v>68.542726879871694</v>
+      </c>
+      <c r="I37" t="s">
+        <v>117</v>
+      </c>
+      <c r="J37" t="s">
+        <v>33</v>
+      </c>
+      <c r="P37" t="s">
+        <v>152</v>
+      </c>
+      <c r="R37" t="b">
+        <v>0</v>
+      </c>
+      <c r="T37" t="b">
+        <v>1</v>
+      </c>
+      <c r="W37" t="s">
+        <v>288</v>
+      </c>
+      <c r="AD37" t="b">
+        <v>1</v>
+      </c>
+      <c r="AE37" t="b">
+        <v>1</v>
+      </c>
+      <c r="AF37" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH37" t="s">
+        <v>289</v>
+      </c>
+      <c r="AI37" t="s">
+        <v>290</v>
+      </c>
+      <c r="AJ37" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="AL37" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="38" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>292</v>
+      </c>
+      <c r="B38" t="s">
+        <v>295</v>
+      </c>
+      <c r="C38" t="s">
+        <v>296</v>
+      </c>
+      <c r="D38" t="s">
+        <v>36</v>
+      </c>
+      <c r="E38">
+        <v>24.248468102019199</v>
+      </c>
+      <c r="F38">
+        <v>67.726593792750194</v>
+      </c>
+      <c r="I38" t="s">
+        <v>297</v>
+      </c>
+      <c r="J38" t="s">
+        <v>33</v>
+      </c>
+      <c r="P38" t="s">
+        <v>152</v>
+      </c>
+      <c r="T38" t="b">
+        <v>1</v>
+      </c>
+      <c r="W38" t="s">
+        <v>298</v>
+      </c>
+      <c r="AD38" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH38" t="s">
+        <v>299</v>
+      </c>
+      <c r="AI38" t="s">
+        <v>290</v>
+      </c>
+      <c r="AJ38" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="AL38" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="39" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>294</v>
+      </c>
+      <c r="B39" t="s">
+        <v>74</v>
+      </c>
+      <c r="C39" t="s">
+        <v>73</v>
+      </c>
+      <c r="D39" t="s">
+        <v>36</v>
+      </c>
+      <c r="E39">
+        <v>24.700069031112299</v>
+      </c>
+      <c r="F39">
+        <v>70.177657039311001</v>
+      </c>
+      <c r="I39" t="s">
+        <v>301</v>
+      </c>
+      <c r="J39" t="s">
+        <v>33</v>
+      </c>
+      <c r="M39">
+        <v>14</v>
+      </c>
+      <c r="P39" t="s">
+        <v>152</v>
+      </c>
+      <c r="AD39" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI39" t="s">
+        <v>290</v>
+      </c>
+      <c r="AJ39" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="AL39" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="40" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>300</v>
+      </c>
+      <c r="B40" t="s">
+        <v>307</v>
+      </c>
+      <c r="C40" t="s">
+        <v>284</v>
+      </c>
+      <c r="D40" t="s">
+        <v>36</v>
+      </c>
+      <c r="E40">
+        <v>27.517261775755902</v>
+      </c>
+      <c r="F40">
+        <v>69.043115588859393</v>
+      </c>
+      <c r="I40" t="s">
+        <v>304</v>
+      </c>
+      <c r="P40" t="s">
+        <v>152</v>
+      </c>
+      <c r="AD40" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI40" t="s">
+        <v>290</v>
+      </c>
+      <c r="AJ40" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="AL40" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="41" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>302</v>
+      </c>
+      <c r="B41" t="s">
+        <v>307</v>
+      </c>
+      <c r="C41" t="s">
+        <v>284</v>
+      </c>
+      <c r="D41" t="s">
+        <v>36</v>
+      </c>
+      <c r="E41">
+        <v>27.517261775755902</v>
+      </c>
+      <c r="F41">
+        <v>69.043115588859393</v>
+      </c>
+      <c r="I41" t="s">
+        <v>306</v>
+      </c>
+      <c r="P41" t="s">
+        <v>152</v>
+      </c>
+      <c r="AD41" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI41" t="s">
+        <v>290</v>
+      </c>
+      <c r="AJ41" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="AL41" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="42" spans="1:38" ht="102" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>303</v>
+      </c>
+      <c r="B42" t="s">
+        <v>310</v>
+      </c>
+      <c r="C42" t="s">
+        <v>268</v>
+      </c>
+      <c r="D42" t="s">
+        <v>36</v>
+      </c>
+      <c r="E42">
+        <v>25.3955393010406</v>
+      </c>
+      <c r="F42">
+        <v>68.354054570775205</v>
+      </c>
+      <c r="G42" s="2">
+        <v>44904</v>
+      </c>
+      <c r="I42" t="s">
+        <v>309</v>
+      </c>
+      <c r="J42" t="s">
+        <v>56</v>
+      </c>
+      <c r="M42">
+        <v>15</v>
+      </c>
+      <c r="P42" t="s">
+        <v>152</v>
+      </c>
+      <c r="R42" t="b">
+        <v>1</v>
+      </c>
+      <c r="S42" t="b">
+        <v>1</v>
+      </c>
+      <c r="W42" t="s">
+        <v>311</v>
+      </c>
+      <c r="AD42" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH42" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="AI42" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ42" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="AL42" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="1:38" ht="136" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>308</v>
+      </c>
+      <c r="B43" t="s">
+        <v>62</v>
+      </c>
+      <c r="C43" t="s">
+        <v>39</v>
+      </c>
+      <c r="D43" t="s">
+        <v>36</v>
+      </c>
+      <c r="E43">
+        <v>25.1805320149683</v>
+      </c>
+      <c r="F43">
+        <v>69.561260523102604</v>
+      </c>
+      <c r="G43" s="2">
+        <v>44904</v>
+      </c>
+      <c r="I43" t="s">
+        <v>315</v>
+      </c>
+      <c r="J43" t="s">
+        <v>76</v>
+      </c>
+      <c r="P43" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>180</v>
+      </c>
+      <c r="S43" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y43" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD43" t="b">
+        <v>1</v>
+      </c>
+      <c r="AE43" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH43" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="AI43" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ43" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="AL43" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="44" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>314</v>
+      </c>
+      <c r="C44" t="s">
+        <v>85</v>
+      </c>
+      <c r="D44" t="s">
+        <v>36</v>
+      </c>
+      <c r="E44">
+        <v>25.5104918059418</v>
+      </c>
+      <c r="F44">
+        <v>69.010155034613007</v>
+      </c>
+      <c r="G44" s="2">
+        <v>44900</v>
+      </c>
+      <c r="I44" t="s">
+        <v>319</v>
+      </c>
+      <c r="J44" t="s">
+        <v>320</v>
+      </c>
+      <c r="P44" t="s">
+        <v>155</v>
+      </c>
+      <c r="R44" t="b">
+        <v>0</v>
+      </c>
+      <c r="S44" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y44" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD44" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH44" t="s">
+        <v>321</v>
+      </c>
+      <c r="AI44" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ44" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="AL44" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="45" spans="1:38" ht="102" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>318</v>
+      </c>
+      <c r="B45" t="s">
+        <v>330</v>
+      </c>
+      <c r="C45" t="s">
+        <v>35</v>
+      </c>
+      <c r="D45" t="s">
+        <v>36</v>
+      </c>
+      <c r="E45">
+        <v>24.7885253117392</v>
+      </c>
+      <c r="F45">
+        <v>68.965730390166996</v>
+      </c>
+      <c r="G45" s="2">
+        <v>44891</v>
+      </c>
+      <c r="I45" t="s">
+        <v>305</v>
+      </c>
+      <c r="J45" t="s">
+        <v>333</v>
+      </c>
+      <c r="P45" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>180</v>
+      </c>
+      <c r="S45" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y45" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD45" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH45" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="AI45" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ45" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="AL45" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="46" spans="1:38" ht="136" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>323</v>
+      </c>
+      <c r="B46" t="s">
+        <v>336</v>
+      </c>
+      <c r="C46" t="s">
+        <v>85</v>
+      </c>
+      <c r="D46" t="s">
+        <v>36</v>
+      </c>
+      <c r="E46">
+        <v>25.285883991678801</v>
+      </c>
+      <c r="F46">
+        <v>69.255448181064807</v>
+      </c>
+      <c r="G46" s="2">
+        <v>44891</v>
+      </c>
+      <c r="I46" t="s">
+        <v>335</v>
+      </c>
+      <c r="J46" t="s">
+        <v>33</v>
+      </c>
+      <c r="P46" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>180</v>
+      </c>
+      <c r="R46" t="b">
+        <v>0</v>
+      </c>
+      <c r="S46" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y46" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB46" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD46" t="b">
+        <v>1</v>
+      </c>
+      <c r="AE46" t="b">
+        <v>1</v>
+      </c>
+      <c r="AF46" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH46" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="AI46" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ46" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="AL46" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="47" spans="1:38" ht="153" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>341</v>
+      </c>
+      <c r="B47" t="s">
+        <v>62</v>
+      </c>
+      <c r="C47" t="s">
+        <v>39</v>
+      </c>
+      <c r="D47" t="s">
+        <v>36</v>
+      </c>
+      <c r="E47">
+        <v>25.178124086636799</v>
+      </c>
+      <c r="F47">
+        <v>69.560831369692295</v>
+      </c>
+      <c r="G47" s="2">
+        <v>44890</v>
+      </c>
+      <c r="I47" t="s">
+        <v>342</v>
+      </c>
+      <c r="J47" t="s">
+        <v>343</v>
+      </c>
+      <c r="P47" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>110</v>
+      </c>
+      <c r="R47" t="b">
+        <v>0</v>
+      </c>
+      <c r="S47" t="b">
+        <v>0</v>
+      </c>
+      <c r="T47" t="b">
+        <v>1</v>
+      </c>
+      <c r="U47" t="b">
+        <v>1</v>
+      </c>
+      <c r="V47" t="s">
+        <v>110</v>
+      </c>
+      <c r="W47" t="s">
+        <v>340</v>
+      </c>
+      <c r="Y47" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB47" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD47" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH47" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="AI47" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ47" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="AL47" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="48" spans="1:38" ht="170" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>344</v>
+      </c>
+      <c r="B48" t="s">
+        <v>345</v>
+      </c>
+      <c r="C48" t="s">
+        <v>73</v>
+      </c>
+      <c r="D48" t="s">
+        <v>36</v>
+      </c>
+      <c r="E48">
+        <v>24.743912457131401</v>
+      </c>
+      <c r="F48">
+        <v>69.806400998791403</v>
+      </c>
+      <c r="I48" t="s">
+        <v>346</v>
+      </c>
+      <c r="J48" t="s">
+        <v>76</v>
+      </c>
+      <c r="P48" t="s">
+        <v>155</v>
+      </c>
+      <c r="T48" t="b">
+        <v>1</v>
+      </c>
+      <c r="W48" t="s">
+        <v>358</v>
+      </c>
+      <c r="Y48" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z48" t="s">
+        <v>90</v>
+      </c>
+      <c r="AA48" t="s">
+        <v>357</v>
+      </c>
+      <c r="AB48" t="b">
+        <v>1</v>
+      </c>
+      <c r="AC48" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD48" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH48" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="AI48" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ48" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="AK48" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="AL48" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="49" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>348</v>
+      </c>
+      <c r="B49" t="s">
+        <v>349</v>
+      </c>
+      <c r="C49" t="s">
+        <v>39</v>
+      </c>
+      <c r="D49" t="s">
+        <v>36</v>
+      </c>
+      <c r="E49">
+        <v>25.511479788435501</v>
+      </c>
+      <c r="F49">
+        <v>69.377192279353196</v>
+      </c>
+      <c r="I49" t="s">
+        <v>350</v>
+      </c>
+      <c r="J49" t="s">
+        <v>76</v>
+      </c>
+      <c r="K49" t="s">
+        <v>351</v>
+      </c>
+      <c r="M49">
+        <v>17</v>
+      </c>
+      <c r="P49" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>180</v>
+      </c>
+      <c r="R49" t="b">
+        <v>1</v>
+      </c>
+      <c r="T49" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y49" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB49" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD49" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI49" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ49" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="AL49" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="50" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>352</v>
+      </c>
+      <c r="B50" t="s">
+        <v>353</v>
+      </c>
+      <c r="C50" t="s">
+        <v>85</v>
+      </c>
+      <c r="D50" t="s">
+        <v>36</v>
+      </c>
+      <c r="E50">
+        <v>24.969018495630099</v>
+      </c>
+      <c r="F50">
+        <v>69.294060335015104</v>
+      </c>
+      <c r="G50" s="2">
+        <v>44831</v>
+      </c>
+      <c r="I50" t="s">
+        <v>354</v>
+      </c>
+      <c r="J50" t="s">
+        <v>381</v>
+      </c>
+      <c r="P50" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>180</v>
+      </c>
+      <c r="R50" t="b">
+        <v>1</v>
+      </c>
+      <c r="T50" t="b">
+        <v>1</v>
+      </c>
+      <c r="W50" t="s">
+        <v>382</v>
+      </c>
+      <c r="Y50" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB50" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD50" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI50" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ50" s="5" t="s">
+        <v>383</v>
+      </c>
+      <c r="AL50" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="51" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>355</v>
+      </c>
+      <c r="B51" t="s">
+        <v>361</v>
+      </c>
+      <c r="C51" t="s">
+        <v>85</v>
+      </c>
+      <c r="D51" t="s">
+        <v>36</v>
+      </c>
+      <c r="E51">
+        <v>25.049148653700101</v>
+      </c>
+      <c r="F51">
+        <v>68.951911936509504</v>
+      </c>
+      <c r="I51" t="s">
+        <v>356</v>
+      </c>
+      <c r="J51" t="s">
+        <v>56</v>
+      </c>
+      <c r="P51" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>180</v>
+      </c>
+      <c r="T51" t="b">
+        <v>1</v>
+      </c>
+      <c r="W51" t="s">
+        <v>362</v>
+      </c>
+      <c r="Y51" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB51" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD51" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI51" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ51" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="AL51" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="52" spans="1:38" ht="153" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>363</v>
+      </c>
+      <c r="B52" t="s">
+        <v>365</v>
+      </c>
+      <c r="C52" t="s">
+        <v>73</v>
+      </c>
+      <c r="D52" t="s">
+        <v>36</v>
+      </c>
+      <c r="E52">
+        <v>24.358531079560901</v>
+      </c>
+      <c r="F52">
+        <v>70.755504609789</v>
+      </c>
+      <c r="G52" s="2">
+        <v>44886</v>
+      </c>
+      <c r="I52" t="s">
+        <v>364</v>
+      </c>
+      <c r="J52" t="s">
+        <v>366</v>
+      </c>
+      <c r="P52" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>180</v>
+      </c>
+      <c r="T52" t="b">
+        <v>1</v>
+      </c>
+      <c r="W52" t="s">
+        <v>367</v>
+      </c>
+      <c r="Y52" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB52" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD52" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH52" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="AI52" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ52" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="AK52" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="AL52" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="53" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>370</v>
+      </c>
+      <c r="B53" t="s">
+        <v>236</v>
+      </c>
+      <c r="C53" t="s">
+        <v>237</v>
+      </c>
+      <c r="D53" t="s">
+        <v>36</v>
+      </c>
+      <c r="E53">
+        <v>28.250621225691599</v>
+      </c>
+      <c r="F53">
+        <v>69.180585555158899</v>
+      </c>
+      <c r="I53" t="s">
+        <v>371</v>
+      </c>
+      <c r="J53" t="s">
+        <v>76</v>
+      </c>
+      <c r="P53" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q53" t="s">
+        <v>180</v>
+      </c>
+      <c r="T53" t="b">
+        <v>1</v>
+      </c>
+      <c r="W53" t="s">
+        <v>372</v>
+      </c>
+      <c r="Y53" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB53" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD53" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH53" t="s">
+        <v>373</v>
+      </c>
+      <c r="AI53" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ53" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="AL53" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="54" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>385</v>
+      </c>
+      <c r="B54" t="s">
+        <v>386</v>
+      </c>
+      <c r="C54" t="s">
+        <v>387</v>
+      </c>
+      <c r="D54" t="s">
+        <v>36</v>
+      </c>
+      <c r="E54">
+        <v>26.466689709855402</v>
+      </c>
+      <c r="F54">
+        <v>67.845934573462898</v>
+      </c>
+      <c r="I54" t="s">
+        <v>388</v>
+      </c>
+      <c r="P54" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>180</v>
+      </c>
+      <c r="T54" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y54" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA54" t="s">
+        <v>244</v>
+      </c>
+      <c r="AC54" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD54" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI54" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ54" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="AL54" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="55" spans="1:38" ht="136" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>389</v>
+      </c>
+      <c r="B55" t="s">
+        <v>336</v>
+      </c>
+      <c r="C55" t="s">
+        <v>85</v>
+      </c>
+      <c r="D55" t="s">
+        <v>36</v>
+      </c>
+      <c r="E55">
+        <v>25.285573563038401</v>
+      </c>
+      <c r="F55">
+        <v>69.254203636174907</v>
+      </c>
+      <c r="G55" s="2">
+        <v>44850</v>
+      </c>
+      <c r="I55" t="s">
+        <v>390</v>
+      </c>
+      <c r="J55" t="s">
+        <v>395</v>
+      </c>
+      <c r="K55" t="s">
+        <v>391</v>
+      </c>
+      <c r="L55" t="s">
+        <v>392</v>
+      </c>
+      <c r="P55" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q55" t="s">
+        <v>180</v>
+      </c>
+      <c r="T55" t="b">
+        <v>1</v>
+      </c>
+      <c r="W55" t="s">
+        <v>396</v>
+      </c>
+      <c r="Y55" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD55" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH55" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="AI55" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ55" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="AK55" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="AL55" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="56" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>397</v>
+      </c>
+      <c r="B56" t="s">
+        <v>398</v>
+      </c>
+      <c r="C56" t="s">
+        <v>73</v>
+      </c>
+      <c r="D56" t="s">
+        <v>36</v>
+      </c>
+      <c r="E56">
+        <v>24.522713721861798</v>
+      </c>
+      <c r="F56">
+        <v>70.368061547807699</v>
+      </c>
+      <c r="G56" s="2">
+        <v>44885</v>
+      </c>
+      <c r="J56" t="s">
+        <v>33</v>
+      </c>
+      <c r="P56" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q56" t="s">
+        <v>180</v>
+      </c>
+      <c r="T56" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y56" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD56" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI56" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ56" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="AL56" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="57" spans="1:38" ht="136" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>402</v>
+      </c>
+      <c r="B57" t="s">
+        <v>407</v>
+      </c>
+      <c r="C57" t="s">
+        <v>408</v>
+      </c>
+      <c r="D57" t="s">
+        <v>36</v>
+      </c>
+      <c r="E57">
+        <v>27.306206500006699</v>
+      </c>
+      <c r="F57">
+        <v>68.614394330533102</v>
+      </c>
+      <c r="G57" s="2">
+        <v>44848</v>
+      </c>
+      <c r="I57" t="s">
+        <v>403</v>
+      </c>
+      <c r="J57" t="s">
+        <v>404</v>
+      </c>
+      <c r="P57" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>180</v>
+      </c>
+      <c r="AD57" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH57" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="AI57" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ57" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="AL57" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:AL28" xr:uid="{7D2FE676-F03D-4E4C-8907-AA9304B213EE}"/>
+  <autoFilter ref="A1:AL56" xr:uid="{7D2FE676-F03D-4E4C-8907-AA9304B213EE}"/>
   <hyperlinks>
     <hyperlink ref="AJ3" r:id="rId1" xr:uid="{7D36CF03-D602-604F-9081-06B44641DFED}"/>
     <hyperlink ref="AJ4" r:id="rId2" xr:uid="{BACCB937-A5FB-A547-AC6D-BEE6543D6916}"/>
@@ -3354,8 +5401,8 @@
     <hyperlink ref="AJ15" r:id="rId15" xr:uid="{A3F6E89E-F629-4D4A-987B-0B2CFFAE4A08}"/>
     <hyperlink ref="AJ16" r:id="rId16" xr:uid="{D18A77C4-9BC3-1648-BCFF-7EEAB9CA9C10}"/>
     <hyperlink ref="AJ17" r:id="rId17" xr:uid="{412E0A2F-A7E5-0242-BF54-576907214B6B}"/>
-    <hyperlink ref="AJ18" r:id="rId18" xr:uid="{E9C71734-E2C4-A141-A43E-CD156CA31D83}"/>
-    <hyperlink ref="AK17" r:id="rId19" xr:uid="{3220CCA7-2920-8843-85A8-00C4A73BC4A8}"/>
+    <hyperlink ref="AJ18" r:id="rId18" display="https://twitter.com/NarainDasBheel8/status/1613879349765181440?s=20&amp;t=EqQ5jcnK36bzUJy8PuZbAg" xr:uid="{E9C71734-E2C4-A141-A43E-CD156CA31D83}"/>
+    <hyperlink ref="AK17" r:id="rId19" display="https://twitter.com/NarainDasBheel8/status/1613880668957573121?s=20&amp;t=EqQ5jcnK36bzUJy8PuZbAg" xr:uid="{3220CCA7-2920-8843-85A8-00C4A73BC4A8}"/>
     <hyperlink ref="AK16" r:id="rId20" xr:uid="{402113FA-8A02-FD4E-931D-6A0670EFE294}"/>
     <hyperlink ref="AJ19" r:id="rId21" xr:uid="{26BE1506-3D2F-7544-86B5-1D44633BF9DD}"/>
     <hyperlink ref="AJ20" r:id="rId22" xr:uid="{1A763510-0993-6849-8881-3659C0A38EA6}"/>
@@ -3375,6 +5422,37 @@
     <hyperlink ref="AJ29" r:id="rId36" xr:uid="{7946EAB1-D298-F840-A38D-972694831ED6}"/>
     <hyperlink ref="AJ30" r:id="rId37" xr:uid="{EC2AABED-B9A1-C943-A741-E6674D4728A1}"/>
     <hyperlink ref="AJ31" r:id="rId38" xr:uid="{3D29D2E0-B4C2-AE4E-849E-DB4C172A3650}"/>
+    <hyperlink ref="AJ32" r:id="rId39" xr:uid="{7ACFE55E-B233-934C-B9F6-7312B9C77A55}"/>
+    <hyperlink ref="AJ33" r:id="rId40" xr:uid="{3D160C8F-D6DB-0B40-B391-E7CC60A56BD3}"/>
+    <hyperlink ref="AJ34" r:id="rId41" xr:uid="{3E246DB4-E25A-6345-A770-3A01CD635880}"/>
+    <hyperlink ref="AJ35" r:id="rId42" xr:uid="{A0C0324C-D7AC-2C41-8410-F248EC205969}"/>
+    <hyperlink ref="AJ36" r:id="rId43" xr:uid="{EE1B2AE4-A6B2-1748-B51E-933BF6DA321E}"/>
+    <hyperlink ref="AJ37" r:id="rId44" xr:uid="{7D8DF362-67D8-014D-8E15-30E6346A6804}"/>
+    <hyperlink ref="AJ38" r:id="rId45" xr:uid="{E4DCAE3A-4FE7-FB48-85F4-6F2CC83117A7}"/>
+    <hyperlink ref="AJ40" r:id="rId46" xr:uid="{7664B802-ADA0-FC4D-9157-05D20523D50B}"/>
+    <hyperlink ref="AJ41" r:id="rId47" xr:uid="{51C8B01E-2FFF-5444-8E75-6AFB674A614E}"/>
+    <hyperlink ref="AJ42" r:id="rId48" xr:uid="{6C6EA9CB-F745-E24A-AB85-81396ED43E1B}"/>
+    <hyperlink ref="AJ43" r:id="rId49" xr:uid="{4E2A60A8-C20D-B74D-8BC9-465DA0EFFD40}"/>
+    <hyperlink ref="AJ44" r:id="rId50" xr:uid="{59C3E9D2-229C-EF45-B566-49AAF5142C8C}"/>
+    <hyperlink ref="AK4" r:id="rId51" xr:uid="{3245D2E9-D48A-7A46-962A-56663778F9EA}"/>
+    <hyperlink ref="AJ39" r:id="rId52" xr:uid="{C5E42DFA-D3E2-4C45-A43F-68E8F732885C}"/>
+    <hyperlink ref="AJ45" r:id="rId53" xr:uid="{E1EDB942-8797-C346-8128-F544492A8F84}"/>
+    <hyperlink ref="AJ46" r:id="rId54" xr:uid="{B99D6161-832D-D84E-8F38-21A95610873A}"/>
+    <hyperlink ref="AJ47" r:id="rId55" xr:uid="{59B7A97D-B771-1048-87C0-8CD2D8929318}"/>
+    <hyperlink ref="AJ48" r:id="rId56" xr:uid="{6A21C941-E8CD-914F-ACBC-2DD6852BDAE5}"/>
+    <hyperlink ref="AJ49" r:id="rId57" xr:uid="{B0F0E028-D272-3949-B9DD-13C9B0768B30}"/>
+    <hyperlink ref="AJ50" r:id="rId58" display="https://twitter.com/NarainDasBheel8/status/1595317492171345921?s=20&amp;t=37g10exefm4l7cU-JhUmkg" xr:uid="{26F90516-54CE-BD49-8F64-A05C7F5B40F5}"/>
+    <hyperlink ref="AJ51" r:id="rId59" xr:uid="{97EA0CAA-98B1-B444-943C-B21EFB71AFAF}"/>
+    <hyperlink ref="AK48" r:id="rId60" xr:uid="{63A5FDA6-95A9-5649-9C92-534C998A6E6C}"/>
+    <hyperlink ref="AJ52" r:id="rId61" xr:uid="{7C6683F3-99F4-D941-AF2F-B0A6AD052FC1}"/>
+    <hyperlink ref="AK52" r:id="rId62" xr:uid="{9A9D1F5C-76AE-D840-AB09-418DA5D6D903}"/>
+    <hyperlink ref="AJ53" r:id="rId63" xr:uid="{D33B5C6B-0882-5040-84AF-5BDA1BBD5AC4}"/>
+    <hyperlink ref="AK33" r:id="rId64" xr:uid="{1BA1533D-E75D-994D-890C-32EBAF2A4018}"/>
+    <hyperlink ref="AJ54" r:id="rId65" xr:uid="{D2BB9451-3364-1045-A6A4-D8E69777A81F}"/>
+    <hyperlink ref="AK55" r:id="rId66" xr:uid="{7CD51FFE-2865-C24F-9A8E-EB416AF4CCB1}"/>
+    <hyperlink ref="AJ55" r:id="rId67" xr:uid="{C8A2366A-AB63-334D-BC85-63BB4625E1AD}"/>
+    <hyperlink ref="AJ56" r:id="rId68" xr:uid="{63404FAC-1C8A-4543-B7FA-9939801864E0}"/>
+    <hyperlink ref="AJ57" r:id="rId69" xr:uid="{FC0391D8-5F1A-C545-9994-D93F3B49CA98}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>